<commit_message>
Unit Tests for RequestHandlers, moved certain Utils from http-endpoint to core
</commit_message>
<xml_diff>
--- a/documentation/mappings/http2request_mapping.xlsx
+++ b/documentation/mappings/http2request_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schick\Documents\Projekte\FA3ST\documentation\mappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schick\Documents\Projekte\FA3ST-Service\documentation\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB91E7C7-7120-4E54-97C9-A7EF32EF86E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBDC58C-75C7-48AE-A240-546751B370C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="8925" xr2:uid="{418FEE22-B724-4565-8C4B-86FBBB26DE63}"/>
   </bookViews>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B775D4E2-0610-4798-A52B-306519969D70}">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>